<commit_message>
Create cinematics at boss spawn
</commit_message>
<xml_diff>
--- a/Data/BonusData.xlsx
+++ b/Data/BonusData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BroGame\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01D819C-DA8C-4858-B034-805EFB56B2EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7B281D-EE24-470A-AB3A-566E3BB1EDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{85F11096-AC3F-4D9D-B598-BE09DDB71694}"/>
+    <workbookView xWindow="4290" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{85F11096-AC3F-4D9D-B598-BE09DDB71694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,14 +98,6 @@
   </si>
   <si>
     <t>Legend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack Up</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -482,7 +474,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -628,16 +620,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -645,16 +637,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -662,16 +654,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -679,16 +671,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -696,16 +688,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -713,16 +705,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -730,16 +722,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
+      <c r="E14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -747,16 +739,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
+      <c r="E15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -764,16 +756,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>7</v>
+      <c r="E16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,16 +773,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>7</v>
+      <c r="E17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -798,16 +790,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>7</v>
+      <c r="E18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -815,16 +807,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>300</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>7</v>
+      <c r="E19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -832,16 +824,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -849,119 +841,35 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>50</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>